<commit_message>
new regression .py files, updated readme
</commit_message>
<xml_diff>
--- a/data for jan 27th.xlsx
+++ b/data for jan 27th.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Google Drive/Tulane/Job stuff/Portfolio Projects/SAT-and-College-GPA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA6E90A-7A0E-684B-AEC0-5A3E99EA4B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F5DD23-4C6C-354C-9479-5CA56E066FAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="1220" windowWidth="28800" windowHeight="15640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my_data" sheetId="15" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
   <si>
     <t>SAT</t>
   </si>
@@ -528,15 +528,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082AE71B-DF39-AE4E-B598-F508BBE3D32B}">
-  <dimension ref="A1:O3111"/>
+  <dimension ref="A1:X3111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:17">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -550,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:17">
       <c r="A2" s="6">
         <v>920</v>
       </c>
@@ -564,7 +564,7 @@
         <v>2.04</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:17">
       <c r="A3" s="6">
         <v>1170</v>
       </c>
@@ -578,7 +578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:17">
       <c r="A4" s="6">
         <v>810</v>
       </c>
@@ -592,7 +592,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:17">
       <c r="A5" s="6">
         <v>940</v>
       </c>
@@ -606,7 +606,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:17">
       <c r="A6" s="6">
         <v>1180</v>
       </c>
@@ -620,7 +620,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:17">
       <c r="A7" s="6">
         <v>980</v>
       </c>
@@ -634,7 +634,7 @@
         <v>3.03</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:17">
       <c r="A8" s="6">
         <v>880</v>
       </c>
@@ -647,11 +647,14 @@
       <c r="D8" s="6">
         <v>1.84</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="16" thickBot="1">
+      <c r="P8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="16" thickBot="1">
       <c r="A9" s="6">
         <v>980</v>
       </c>
@@ -665,7 +668,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:17">
       <c r="A10" s="6">
         <v>1240</v>
       </c>
@@ -678,12 +681,16 @@
       <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="G10" s="4"/>
+      <c r="P10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="6">
         <v>1230</v>
       </c>
@@ -696,14 +703,20 @@
       <c r="D11" s="6">
         <v>2</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="1">
+      <c r="G11" s="1">
+        <v>0.41124114212477841</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="1">
         <v>0.44160636287888999</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:17">
       <c r="A12" s="6">
         <v>1140</v>
       </c>
@@ -716,14 +729,20 @@
       <c r="D12" s="6">
         <v>2.98</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="1">
+      <c r="G12" s="1">
+        <v>0.16911927697609222</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q12" s="1">
         <v>0.19501617973512189</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:17">
       <c r="A13" s="6">
         <v>1150</v>
       </c>
@@ -736,14 +755,20 @@
       <c r="D13" s="6">
         <v>2.93</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="1">
+      <c r="G13" s="1">
+        <v>0.16885194083612315</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="1">
         <v>0.19423866799629555</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:17">
       <c r="A14" s="6">
         <v>1080</v>
       </c>
@@ -756,14 +781,20 @@
       <c r="D14" s="6">
         <v>2</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="1">
+      <c r="G14" s="1">
+        <v>0.59321754767396151</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="1">
         <v>0.58408762187731744</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16" thickBot="1">
+    <row r="15" spans="1:17" ht="16" thickBot="1">
       <c r="A15" s="6">
         <v>990</v>
       </c>
@@ -776,14 +807,20 @@
       <c r="D15" s="6">
         <v>2.21</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="2">
+      <c r="G15" s="2">
         <v>3110</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="P15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="6">
         <v>1000</v>
       </c>
@@ -797,7 +834,7 @@
         <v>3.33</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="16" thickBot="1">
+    <row r="17" spans="1:24" ht="16" thickBot="1">
       <c r="A17" s="6">
         <v>1050</v>
       </c>
@@ -810,11 +847,14 @@
       <c r="D17" s="6">
         <v>1.07</v>
       </c>
-      <c r="G17" t="s">
+      <c r="F17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18" s="6">
         <v>1160</v>
       </c>
@@ -827,24 +867,40 @@
       <c r="D18" s="6">
         <v>2.29</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="H18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="R18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="S18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="T18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="U18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:24">
       <c r="A19" s="6">
         <v>1190</v>
       </c>
@@ -857,26 +913,44 @@
       <c r="D19" s="6">
         <v>3.15</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
       <c r="H19" s="1">
+        <v>222.61961052282118</v>
+      </c>
+      <c r="I19" s="1">
+        <v>222.61961052282118</v>
+      </c>
+      <c r="J19" s="1">
+        <v>632.60910775344871</v>
+      </c>
+      <c r="K19" s="1">
+        <v>3.191525560123077E-127</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q19" s="1">
         <v>3</v>
       </c>
-      <c r="I19" s="1">
+      <c r="R19" s="1">
         <v>256.70891429141261</v>
       </c>
-      <c r="J19" s="1">
+      <c r="S19" s="1">
         <v>85.569638097137542</v>
       </c>
-      <c r="K19" s="1">
+      <c r="T19" s="1">
         <v>250.8208815335683</v>
       </c>
-      <c r="L19" s="1">
+      <c r="U19" s="1">
         <v>9.576409023214791E-146</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:24">
       <c r="A20" s="6">
         <v>1030</v>
       </c>
@@ -889,22 +963,36 @@
       <c r="D20" s="6">
         <v>2.65</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="G20" s="1">
+        <v>3108</v>
+      </c>
       <c r="H20" s="1">
+        <v>1093.7271389627037</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.35190705886830881</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="P20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q20" s="1">
         <v>3106</v>
       </c>
-      <c r="I20" s="1">
+      <c r="R20" s="1">
         <v>1059.6378351941123</v>
       </c>
-      <c r="J20" s="1">
+      <c r="S20" s="1">
         <v>0.34115835003030015</v>
       </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" ht="16" thickBot="1">
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="1:24" ht="16" thickBot="1">
       <c r="A21" s="6">
         <v>960</v>
       </c>
@@ -917,20 +1005,32 @@
       <c r="D21" s="6">
         <v>2.41</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="G21" s="2">
+        <v>3109</v>
+      </c>
       <c r="H21" s="2">
-        <v>3109</v>
-      </c>
-      <c r="I21" s="2">
         <v>1316.3467494855249</v>
       </c>
+      <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" ht="16" thickBot="1">
+      <c r="P21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>3109</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1316.3467494855249</v>
+      </c>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="1:24" ht="16" thickBot="1">
       <c r="A22" s="6">
         <v>840</v>
       </c>
@@ -944,7 +1044,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:24">
       <c r="A23" s="6">
         <v>920</v>
       </c>
@@ -957,33 +1057,58 @@
       <c r="D23" s="6">
         <v>2.64</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="H23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="R23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="S23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="T23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="U23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="V23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N23" s="3" t="s">
+      <c r="W23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="X23" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:24">
       <c r="A24" s="6">
         <v>840</v>
       </c>
@@ -996,35 +1121,62 @@
       <c r="D24" s="6">
         <v>2.1800000000000002</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G24" s="1">
+        <v>0.68381495685594018</v>
+      </c>
       <c r="H24" s="1">
+        <v>7.9484879916862636E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>8.6030822160287315</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1.2115415027079176E-17</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.52796676252942454</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.83966315118245582</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0.52796676252942454</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.83966315118245582</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q24" s="1">
         <v>0.4580795155266349</v>
       </c>
-      <c r="I24" s="1">
+      <c r="R24" s="1">
         <v>8.4084160490481868E-2</v>
       </c>
-      <c r="J24" s="1">
+      <c r="S24" s="1">
         <v>5.4478692878011001</v>
       </c>
-      <c r="K24" s="1">
+      <c r="T24" s="1">
         <v>5.4954951917277461E-8</v>
       </c>
-      <c r="L24" s="1">
+      <c r="U24" s="1">
         <v>0.29321334368441054</v>
       </c>
-      <c r="M24" s="1">
+      <c r="V24" s="1">
         <v>0.62294568736885925</v>
       </c>
-      <c r="N24" s="1">
+      <c r="W24" s="1">
         <v>0.29321334368441054</v>
       </c>
-      <c r="O24" s="1">
+      <c r="X24" s="1">
         <v>0.62294568736885925</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:24" ht="16" thickBot="1">
       <c r="A25" s="6">
         <v>1000</v>
       </c>
@@ -1037,35 +1189,62 @@
       <c r="D25" s="6">
         <v>2.84</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1.9219451396116068E-3</v>
+      </c>
+      <c r="H25" s="2">
+        <v>7.6414058550523984E-5</v>
+      </c>
+      <c r="I25" s="2">
+        <v>25.151721765188555</v>
+      </c>
+      <c r="J25" s="2">
+        <v>3.1915255601085396E-127</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1.7721179893571679E-3</v>
+      </c>
+      <c r="L25" s="2">
+        <v>2.0717722898660456E-3</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1.7721179893571679E-3</v>
+      </c>
+      <c r="N25" s="2">
+        <v>2.0717722898660456E-3</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="1">
         <v>2.0455894888062012E-3</v>
       </c>
-      <c r="I25" s="1">
+      <c r="R25" s="1">
         <v>7.8069942228566804E-5</v>
       </c>
-      <c r="J25" s="1">
+      <c r="S25" s="1">
         <v>26.202011048212274</v>
       </c>
-      <c r="K25" s="1">
+      <c r="T25" s="1">
         <v>6.8493280599763064E-137</v>
       </c>
-      <c r="L25" s="1">
+      <c r="U25" s="1">
         <v>1.8925155633951912E-3</v>
       </c>
-      <c r="M25" s="1">
+      <c r="V25" s="1">
         <v>2.1986634142172113E-3</v>
       </c>
-      <c r="N25" s="1">
+      <c r="W25" s="1">
         <v>1.8925155633951912E-3</v>
       </c>
-      <c r="O25" s="1">
+      <c r="X25" s="1">
         <v>2.1986634142172113E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:24">
       <c r="A26" s="6">
         <v>1150</v>
       </c>
@@ -1078,35 +1257,35 @@
       <c r="D26" s="6">
         <v>2.84</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H26" s="1">
+      <c r="Q26" s="1">
         <v>0.21398519060562055</v>
       </c>
-      <c r="I26" s="1">
+      <c r="R26" s="1">
         <v>2.1526962909173254E-2</v>
       </c>
-      <c r="J26" s="1">
+      <c r="S26" s="1">
         <v>9.9403335021511712</v>
       </c>
-      <c r="K26" s="1">
+      <c r="T26" s="1">
         <v>6.0935688573599728E-23</v>
       </c>
-      <c r="L26" s="1">
+      <c r="U26" s="1">
         <v>0.17177667064749247</v>
       </c>
-      <c r="M26" s="1">
+      <c r="V26" s="1">
         <v>0.25619371056374862</v>
       </c>
-      <c r="N26" s="1">
+      <c r="W26" s="1">
         <v>0.17177667064749247</v>
       </c>
-      <c r="O26" s="1">
+      <c r="X26" s="1">
         <v>0.25619371056374862</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="16" thickBot="1">
+    <row r="27" spans="1:24" ht="16" thickBot="1">
       <c r="A27" s="6">
         <v>1040</v>
       </c>
@@ -1119,35 +1298,35 @@
       <c r="D27" s="6">
         <v>2.93</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="P27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="2">
+      <c r="Q27" s="2">
         <v>2.134870245754112E-2</v>
       </c>
-      <c r="I27" s="2">
+      <c r="R27" s="2">
         <v>4.8371779014151156E-2</v>
       </c>
-      <c r="J27" s="2">
+      <c r="S27" s="2">
         <v>0.4413462331268726</v>
       </c>
-      <c r="K27" s="2">
+      <c r="T27" s="2">
         <v>0.65899308103791543</v>
       </c>
-      <c r="L27" s="2">
+      <c r="U27" s="2">
         <v>-7.3495201373357966E-2</v>
       </c>
-      <c r="M27" s="2">
+      <c r="V27" s="2">
         <v>0.11619260628844022</v>
       </c>
-      <c r="N27" s="2">
+      <c r="W27" s="2">
         <v>-7.3495201373357966E-2</v>
       </c>
-      <c r="O27" s="2">
+      <c r="X27" s="2">
         <v>0.11619260628844022</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:24">
       <c r="A28" s="6">
         <v>970</v>
       </c>
@@ -1161,7 +1340,7 @@
         <v>2.29</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:24">
       <c r="A29" s="6">
         <v>1200</v>
       </c>
@@ -1175,7 +1354,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:24">
       <c r="A30" s="6">
         <v>1090</v>
       </c>
@@ -1189,7 +1368,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:24">
       <c r="A31" s="6">
         <v>1340</v>
       </c>
@@ -1203,7 +1382,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:24">
       <c r="A32" s="6">
         <v>740</v>
       </c>

</xml_diff>